<commit_message>
Updated plans for Marketing
Updated plans for Marketing
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/Dec2023/SchoolVisitPlan.xlsx
+++ b/Offline/BusinessManagement/Marketing/Dec2023/SchoolVisitPlan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Anodiam\docs\Offline\BusinessManagement\Marketing\Dec2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\Dec2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A17028B-4AF9-403E-A6CC-6199BC909EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" tabRatio="540"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily-Marketing-Plan" sheetId="7" r:id="rId1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>del</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>CBSE</t>
   </si>
@@ -166,12 +167,36 @@
   </si>
   <si>
     <t>Vivekananda, Baruipur</t>
+  </si>
+  <si>
+    <t>Calcutta Public School</t>
+  </si>
+  <si>
+    <t>St. Ignatius</t>
+  </si>
+  <si>
+    <t>Young Horizon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swarnim </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lion's </t>
+  </si>
+  <si>
+    <t>John Bosco</t>
+  </si>
+  <si>
+    <t>St Stephens</t>
+  </si>
+  <si>
+    <t>AG Tollygunj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -222,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -233,7 +258,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -252,9 +276,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Debashish Nath" id="{4666E732-BD10-4E5E-A636-505584664154}" userId="821c4797ba281e6e" providerId="Windows Live"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,29 +541,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="1" customWidth="1"/>
     <col min="8" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="19.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -585,7 +605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -596,11 +616,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -608,16 +628,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -625,7 +645,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -633,7 +653,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -641,7 +661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -649,7 +669,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -657,7 +677,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -665,7 +685,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -673,7 +693,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -681,7 +701,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -689,7 +709,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -697,7 +717,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -705,7 +725,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -713,7 +733,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -721,7 +741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -729,7 +749,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -740,7 +760,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -748,12 +768,55 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update School Visit Plan
Update School Visit Plan
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/Dec2023/SchoolVisitPlan.xlsx
+++ b/Offline/BusinessManagement/Marketing/Dec2023/SchoolVisitPlan.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\Dec2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A17028B-4AF9-403E-A6CC-6199BC909EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D571D7C3-8E5D-4F76-AD64-6E4273115142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily-Marketing-Plan" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -247,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -257,6 +266,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -273,10 +285,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -544,12 +552,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" bestFit="1" customWidth="1"/>
@@ -606,7 +616,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -616,12 +626,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-    </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -629,7 +635,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -638,7 +644,7 @@
       <c r="G5"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -646,7 +652,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -654,7 +660,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -662,7 +668,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -670,7 +676,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -678,7 +684,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -686,7 +692,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -694,7 +700,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -702,7 +708,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -710,7 +716,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -718,7 +724,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -726,7 +732,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -734,7 +740,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -742,7 +748,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -750,7 +756,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -761,7 +767,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -769,7 +775,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -777,45 +783,66 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+      <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
+      <c r="A24" s="4">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
+      <c r="A26" s="4">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
+      <c r="A27" s="4">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
+      <c r="A28" s="4">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
+      <c r="A29" s="4">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
+      <c r="A30" s="4">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>